<commit_message>
Deploying to gh-pages from  @ a59f070b5266c3a9b4393a5bfe459c5cb24ce8b1 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_5-2-1.xlsx
+++ b/assets/excel/2021_5-2-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06163C2F-C363-4FBA-945B-60D0009AE067}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8E21E5F-C9C8-434E-9666-974A7FD5C7B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{85247E4B-3EF4-475F-BA74-B7C111865EC2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11208" xr2:uid="{85247E4B-3EF4-475F-BA74-B7C111865EC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -456,14 +456,11 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -483,6 +480,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -493,19 +505,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2000,42 +2000,45 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:S54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="5" max="6" width="12.77734375" customWidth="1"/>
+    <col min="10" max="11" width="12.77734375" customWidth="1"/>
+    <col min="15" max="16" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
+    <row r="2" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="2:19" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -2046,127 +2049,127 @@
       <c r="I5" s="4"/>
       <c r="N5" s="6"/>
     </row>
-    <row r="6" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
+    <row r="6" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="24" t="s">
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="24" t="s">
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="26"/>
-    </row>
-    <row r="7" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="34"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="27" t="s">
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="36"/>
+    </row>
+    <row r="7" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="38"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="27" t="s">
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="30" t="s">
+      <c r="J7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="27" t="s">
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="30" t="s">
+      <c r="O7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="32"/>
-    </row>
-    <row r="8" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="34"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="38" t="s">
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="31"/>
+    </row>
+    <row r="8" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="38"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="38" t="s">
+      <c r="H8" s="36"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="39" t="s">
+      <c r="K8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="24" t="s">
+      <c r="L8" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="26"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="38" t="s">
+      <c r="M8" s="36"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="P8" s="39" t="s">
+      <c r="P8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" s="24" t="s">
+      <c r="Q8" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="R8" s="26"/>
-    </row>
-    <row r="9" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="34"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="40"/>
+      <c r="R8" s="36"/>
+    </row>
+    <row r="9" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="38"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="29"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="40"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="34"/>
       <c r="L9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="M9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="29"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="40"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="34"/>
       <c r="Q9" s="7" t="s">
         <v>11</v>
       </c>
@@ -2174,29 +2177,29 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="30" t="s">
+    <row r="10" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="39"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
-      <c r="O10" s="31"/>
-      <c r="P10" s="31"/>
-      <c r="Q10" s="31"/>
-      <c r="R10" s="31"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
       <c r="S10" s="6"/>
     </row>
-    <row r="11" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8">
         <v>1</v>
       </c>
@@ -2250,7 +2253,7 @@
       </c>
       <c r="S11" s="10"/>
     </row>
-    <row r="12" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="11">
         <v>2019</v>
       </c>
@@ -2319,7 +2322,7 @@
       </c>
       <c r="S12" s="10"/>
     </row>
-    <row r="13" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="11">
         <v>2019</v>
       </c>
@@ -2388,7 +2391,7 @@
       </c>
       <c r="S13" s="10"/>
     </row>
-    <row r="14" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11">
         <v>2019</v>
       </c>
@@ -2457,7 +2460,7 @@
       </c>
       <c r="S14" s="10"/>
     </row>
-    <row r="15" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="13">
         <v>2018</v>
       </c>
@@ -2511,7 +2514,7 @@
       </c>
       <c r="S15" s="15"/>
     </row>
-    <row r="16" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="13">
         <v>2018</v>
       </c>
@@ -2565,7 +2568,7 @@
       </c>
       <c r="S16" s="15"/>
     </row>
-    <row r="17" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="13">
         <v>2018</v>
       </c>
@@ -2619,7 +2622,7 @@
       </c>
       <c r="S17" s="15"/>
     </row>
-    <row r="18" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="13">
         <v>2017</v>
       </c>
@@ -2688,7 +2691,7 @@
       </c>
       <c r="S18" s="15"/>
     </row>
-    <row r="19" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="13">
         <v>2017</v>
       </c>
@@ -2757,7 +2760,7 @@
       </c>
       <c r="S19" s="15"/>
     </row>
-    <row r="20" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13">
         <v>2017</v>
       </c>
@@ -2826,7 +2829,7 @@
       </c>
       <c r="S20" s="15"/>
     </row>
-    <row r="21" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="13">
         <v>2016</v>
       </c>
@@ -2895,7 +2898,7 @@
       </c>
       <c r="S21" s="15"/>
     </row>
-    <row r="22" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="13">
         <v>2016</v>
       </c>
@@ -2964,7 +2967,7 @@
       </c>
       <c r="S22" s="15"/>
     </row>
-    <row r="23" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="13">
         <v>2016</v>
       </c>
@@ -3033,7 +3036,7 @@
       </c>
       <c r="S23" s="15"/>
     </row>
-    <row r="24" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="13">
         <v>2015</v>
       </c>
@@ -3102,7 +3105,7 @@
       </c>
       <c r="S24" s="15"/>
     </row>
-    <row r="25" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="13">
         <v>2015</v>
       </c>
@@ -3171,7 +3174,7 @@
       </c>
       <c r="S25" s="15"/>
     </row>
-    <row r="26" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="13">
         <v>2015</v>
       </c>
@@ -3240,7 +3243,7 @@
       </c>
       <c r="S26" s="15"/>
     </row>
-    <row r="27" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="13">
         <v>2014</v>
       </c>
@@ -3309,7 +3312,7 @@
       </c>
       <c r="S27" s="15"/>
     </row>
-    <row r="28" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="13">
         <v>2014</v>
       </c>
@@ -3378,7 +3381,7 @@
       </c>
       <c r="S28" s="15"/>
     </row>
-    <row r="29" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="13">
         <v>2014</v>
       </c>
@@ -3447,7 +3450,7 @@
       </c>
       <c r="S29" s="15"/>
     </row>
-    <row r="30" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="13">
         <v>2013</v>
       </c>
@@ -3516,7 +3519,7 @@
       </c>
       <c r="S30" s="15"/>
     </row>
-    <row r="31" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="13">
         <v>2013</v>
       </c>
@@ -3585,7 +3588,7 @@
       </c>
       <c r="S31" s="15"/>
     </row>
-    <row r="32" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="13">
         <v>2013</v>
       </c>
@@ -3654,7 +3657,7 @@
       </c>
       <c r="S32" s="15"/>
     </row>
-    <row r="33" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="13">
         <v>2012</v>
       </c>
@@ -3723,7 +3726,7 @@
       </c>
       <c r="S33" s="15"/>
     </row>
-    <row r="34" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="13">
         <v>2012</v>
       </c>
@@ -3792,7 +3795,7 @@
       </c>
       <c r="S34" s="15"/>
     </row>
-    <row r="35" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="13">
         <v>2012</v>
       </c>
@@ -3861,7 +3864,7 @@
       </c>
       <c r="S35" s="15"/>
     </row>
-    <row r="36" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="13">
         <v>2011</v>
       </c>
@@ -3930,7 +3933,7 @@
       </c>
       <c r="S36" s="15"/>
     </row>
-    <row r="37" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="13">
         <v>2011</v>
       </c>
@@ -3999,7 +4002,7 @@
       </c>
       <c r="S37" s="15"/>
     </row>
-    <row r="38" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="13">
         <v>2011</v>
       </c>
@@ -4068,7 +4071,7 @@
       </c>
       <c r="S38" s="15"/>
     </row>
-    <row r="39" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="13">
         <v>2005</v>
       </c>
@@ -4122,7 +4125,7 @@
       </c>
       <c r="S39" s="15"/>
     </row>
-    <row r="40" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="13">
         <v>2005</v>
       </c>
@@ -4176,7 +4179,7 @@
       </c>
       <c r="S40" s="15"/>
     </row>
-    <row r="41" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="13">
         <v>2005</v>
       </c>
@@ -4256,19 +4259,19 @@
       <c r="K43" s="18"/>
       <c r="N43" s="19"/>
     </row>
-    <row r="44" spans="2:19" s="20" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="36" t="s">
+    <row r="44" spans="2:19" s="20" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
-      <c r="K44" s="36"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
       <c r="N44" s="21"/>
     </row>
     <row r="45" spans="2:19" s="5" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -4286,35 +4289,35 @@
       <c r="K45" s="18"/>
       <c r="N45" s="19"/>
     </row>
-    <row r="46" spans="2:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="37" t="s">
+    <row r="46" spans="2:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="37"/>
-      <c r="H46" s="37"/>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
-      <c r="K46" s="37"/>
-    </row>
-    <row r="47" spans="2:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="37" t="s">
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
+    </row>
+    <row r="47" spans="2:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37"/>
-      <c r="K47" s="37"/>
-    </row>
-    <row r="48" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24"/>
+      <c r="K47" s="24"/>
+    </row>
+    <row r="48" spans="2:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
       <c r="D48" s="22"/>
@@ -4326,7 +4329,7 @@
       <c r="J48" s="22"/>
       <c r="K48" s="22"/>
     </row>
-    <row r="49" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="18" t="s">
         <v>19</v>
       </c>
@@ -4340,8 +4343,8 @@
       <c r="J49" s="22"/>
       <c r="K49" s="22"/>
     </row>
-    <row r="50" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="18" t="s">
         <v>20</v>
       </c>
@@ -4355,7 +4358,7 @@
       <c r="J51" s="22"/>
       <c r="K51" s="22"/>
     </row>
-    <row r="52" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="18" t="s">
         <v>21</v>
       </c>
@@ -4369,7 +4372,7 @@
       <c r="J52" s="22"/>
       <c r="K52" s="22"/>
     </row>
-    <row r="53" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="18" t="s">
         <v>22</v>
       </c>
@@ -4383,7 +4386,7 @@
       <c r="J53" s="22"/>
       <c r="K53" s="22"/>
     </row>
-    <row r="54" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="23" t="s">
         <v>23</v>
       </c>
@@ -4399,6 +4402,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="D10:R10"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="Q8:R8"/>
     <mergeCell ref="B47:K47"/>
     <mergeCell ref="B44:K44"/>
     <mergeCell ref="B46:K46"/>
@@ -4412,18 +4427,6 @@
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="O8:O9"/>
     <mergeCell ref="P8:P9"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="I6:M6"/>
-    <mergeCell ref="D10:R10"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="Q8:R8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B54" r:id="rId1" xr:uid="{378039AC-FEBF-433F-9CA7-5A8047F9398F}"/>

</xml_diff>